<commit_message>
début réparation assignation jeh url
</commit_message>
<xml_diff>
--- a/Logiciel_PEP/mysite/polls/static/polls/BV_test.xlsx
+++ b/Logiciel_PEP/mysite/polls/static/polls/BV_test.xlsx
@@ -1216,7 +1216,7 @@
         </is>
       </c>
       <c r="I13" s="24" t="n">
-        <v>1080</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="115">
@@ -1236,7 +1236,7 @@
         </is>
       </c>
       <c r="I14" s="27" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="115">

</xml_diff>

<commit_message>
Page details eleve bcp plus fonctionnelle
</commit_message>
<xml_diff>
--- a/Logiciel_PEP/mysite/polls/static/polls/BV_test.xlsx
+++ b/Logiciel_PEP/mysite/polls/static/polls/BV_test.xlsx
@@ -1216,7 +1216,7 @@
         </is>
       </c>
       <c r="I13" s="24" t="n">
-        <v>0</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="115">
@@ -1236,7 +1236,7 @@
         </is>
       </c>
       <c r="I14" s="27" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="115">

</xml_diff>

<commit_message>
ajout des documents, de certains champs, suppression du champs representa nt pour un clien, desormais on ajoute un client, puis au moins un representant et quand on ajoute une mission on selectionne un client, un interlo cuteur client (en gros le gars avait qui la JE echange et un repres. legale (en gros le gars qui signe les papiers)
</commit_message>
<xml_diff>
--- a/Logiciel_PEP/mysite/polls/static/polls/BV_test.xlsx
+++ b/Logiciel_PEP/mysite/polls/static/polls/BV_test.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="H2" s="7" t="inlineStr">
         <is>
-          <t>N° 24027</t>
+          <t>N° 24001</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       <c r="H3" s="8" t="n"/>
       <c r="I3" s="10" t="inlineStr">
         <is>
-          <t>05 février 2024</t>
+          <t>21 July 2024</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="G4" s="12" t="inlineStr">
         <is>
-          <t>Antony FEORD</t>
+          <t>Antony Feord</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="G6" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 rue des Maraichers </t>
+          <t>4 rue des M</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
-          <t>67000 STRASBOURG</t>
+          <t>77420 France</t>
         </is>
       </c>
     </row>
@@ -1188,8 +1188,10 @@
           <t>N° SS :</t>
         </is>
       </c>
-      <c r="H10" s="18" t="n">
-        <v>102116748297847</v>
+      <c r="H10" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="115">
@@ -1207,7 +1209,7 @@
       </c>
       <c r="C13" s="22" t="inlineStr">
         <is>
-          <t>23e41</t>
+          <t>24e01</t>
         </is>
       </c>
       <c r="G13" s="23" t="inlineStr">
@@ -1216,7 +1218,7 @@
         </is>
       </c>
       <c r="I13" s="24" t="n">
-        <v>1080</v>
+        <v>560</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="115">
@@ -1236,7 +1238,7 @@
         </is>
       </c>
       <c r="I14" s="27" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="115">
@@ -1401,7 +1403,7 @@
         <v/>
       </c>
       <c r="F23" s="55" t="n">
-        <v>0.0066</v>
+        <v>0.66</v>
       </c>
       <c r="G23" s="56">
         <f>ROUND(F23*E23,2)</f>

</xml_diff>